<commit_message>
total penalty added to output excel file
</commit_message>
<xml_diff>
--- a/final_finished_solution/large_invigilators.xlsx
+++ b/final_finished_solution/large_invigilators.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nik/July_Git_Repo/final-year-project-NikKontos.2/attempt3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nik/July_Git_Repo/final-year-project-NikKontos.2/final_finished_solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34595E48-3F90-AF4B-A196-C4CF8AF2FBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E16FE-49B3-6A43-9967-D42DF668BA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1040" windowWidth="25040" windowHeight="13620" xr2:uid="{59A6529F-BFDE-4247-92E9-D85FA7B5BB99}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>invig_id</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Abigail Smith</t>
-  </si>
-  <si>
-    <t>s,m,l</t>
   </si>
   <si>
     <t>Alice Johnson</t>
@@ -1369,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9259C063-0089-3041-BBBC-62FD6FFF3990}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1401,13 +1398,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1416,16 +1410,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1434,16 +1425,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1452,16 +1440,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1470,16 +1455,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1488,16 +1470,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1506,16 +1485,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1524,16 +1500,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1542,16 +1515,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1560,16 +1530,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1578,16 +1545,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1596,16 +1560,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1614,16 +1575,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1632,16 +1590,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1650,1096 +1605,913 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>95</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>96</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>97</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>99</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>101</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>102</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>103</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>104</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>105</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>106</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>107</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>108</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>109</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>110</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>111</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>112</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>113</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>114</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>115</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>116</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>117</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>118</v>
       </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>119</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>120</v>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>121</v>
       </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>122</v>
       </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>123</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>124</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
         <v>50</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>125</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
         <v>51</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>126</v>
       </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
         <v>52</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>127</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
         <v>53</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>128</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
         <v>54</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>129</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
         <v>55</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>130</v>
       </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
         <v>56</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>131</v>
       </c>
-      <c r="D52">
-        <v>0</v>
-      </c>
-      <c r="E52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>132</v>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
         <v>58</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>133</v>
       </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
         <v>59</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>134</v>
       </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
         <v>60</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>135</v>
       </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
         <v>61</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>136</v>
       </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
         <v>62</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>137</v>
       </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
         <v>63</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>138</v>
       </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
         <v>64</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>139</v>
       </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>65</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>140</v>
       </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
         <v>66</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>141</v>
       </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
         <v>67</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>142</v>
       </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
         <v>68</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>143</v>
       </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
         <v>69</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>144</v>
       </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C66" t="s">
-        <v>145</v>
-      </c>
       <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" ref="A67:A76" si="1">ROW()-2</f>
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
objective status output to excel (infeasible or optimal) :
</commit_message>
<xml_diff>
--- a/final_finished_solution/large_invigilators.xlsx
+++ b/final_finished_solution/large_invigilators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nik/July_Git_Repo/final-year-project-NikKontos.2/final_finished_solution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145E16FE-49B3-6A43-9967-D42DF668BA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E1041C-A3CB-1E46-9430-8F60097F05CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1040" windowWidth="25040" windowHeight="13620" xr2:uid="{59A6529F-BFDE-4247-92E9-D85FA7B5BB99}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="156">
   <si>
     <t>invig_id</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8,83</t>
+  </si>
+  <si>
+    <t>s,m,l</t>
   </si>
 </sst>
 </file>
@@ -1367,7 +1370,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,6 +1406,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1418,6 +1424,9 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1433,6 +1442,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1448,6 +1460,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1463,6 +1478,9 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1478,6 +1496,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1493,6 +1514,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1508,6 +1532,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1523,6 +1550,9 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1538,6 +1568,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1553,6 +1586,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1568,6 +1604,9 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1583,6 +1622,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1598,6 +1640,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1613,8 +1658,11 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1628,8 +1676,11 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1643,8 +1694,11 @@
       <c r="D18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1658,8 +1712,11 @@
       <c r="D19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1673,8 +1730,11 @@
       <c r="D20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1688,8 +1748,11 @@
       <c r="D21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1703,8 +1766,11 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1718,8 +1784,11 @@
       <c r="D23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1733,8 +1802,11 @@
       <c r="D24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1746,10 +1818,13 @@
         <v>103</v>
       </c>
       <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1761,10 +1836,13 @@
         <v>104</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1776,10 +1854,13 @@
         <v>105</v>
       </c>
       <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1791,10 +1872,13 @@
         <v>106</v>
       </c>
       <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1806,10 +1890,13 @@
         <v>107</v>
       </c>
       <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1821,10 +1908,13 @@
         <v>108</v>
       </c>
       <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1836,10 +1926,13 @@
         <v>109</v>
       </c>
       <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1851,10 +1944,13 @@
         <v>110</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1866,10 +1962,13 @@
         <v>111</v>
       </c>
       <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1881,10 +1980,13 @@
         <v>112</v>
       </c>
       <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1896,10 +1998,13 @@
         <v>113</v>
       </c>
       <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1911,10 +2016,13 @@
         <v>114</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1926,10 +2034,13 @@
         <v>115</v>
       </c>
       <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1941,10 +2052,13 @@
         <v>116</v>
       </c>
       <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1956,10 +2070,13 @@
         <v>117</v>
       </c>
       <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1971,10 +2088,13 @@
         <v>118</v>
       </c>
       <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1986,10 +2106,13 @@
         <v>119</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2001,10 +2124,13 @@
         <v>120</v>
       </c>
       <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2016,10 +2142,13 @@
         <v>121</v>
       </c>
       <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2031,10 +2160,13 @@
         <v>122</v>
       </c>
       <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2046,10 +2178,13 @@
         <v>123</v>
       </c>
       <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2061,10 +2196,13 @@
         <v>124</v>
       </c>
       <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2076,10 +2214,13 @@
         <v>125</v>
       </c>
       <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2091,10 +2232,13 @@
         <v>126</v>
       </c>
       <c r="D48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2106,10 +2250,13 @@
         <v>127</v>
       </c>
       <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2121,10 +2268,13 @@
         <v>128</v>
       </c>
       <c r="D50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2136,10 +2286,13 @@
         <v>129</v>
       </c>
       <c r="D51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2151,10 +2304,13 @@
         <v>130</v>
       </c>
       <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2166,10 +2322,13 @@
         <v>131</v>
       </c>
       <c r="D53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2181,10 +2340,13 @@
         <v>132</v>
       </c>
       <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2196,10 +2358,13 @@
         <v>133</v>
       </c>
       <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2211,10 +2376,13 @@
         <v>134</v>
       </c>
       <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2226,10 +2394,13 @@
         <v>135</v>
       </c>
       <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2241,10 +2412,13 @@
         <v>136</v>
       </c>
       <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2256,10 +2430,13 @@
         <v>137</v>
       </c>
       <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2271,10 +2448,13 @@
         <v>138</v>
       </c>
       <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2286,10 +2466,13 @@
         <v>139</v>
       </c>
       <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2301,10 +2484,13 @@
         <v>140</v>
       </c>
       <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2316,10 +2502,13 @@
         <v>141</v>
       </c>
       <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2331,10 +2520,13 @@
         <v>142</v>
       </c>
       <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2346,10 +2538,13 @@
         <v>143</v>
       </c>
       <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2361,10 +2556,13 @@
         <v>144</v>
       </c>
       <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" ref="A67:A76" si="1">ROW()-2</f>
         <v>65</v>
@@ -2376,10 +2574,13 @@
         <v>145</v>
       </c>
       <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -2391,10 +2592,13 @@
         <v>146</v>
       </c>
       <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -2406,10 +2610,13 @@
         <v>147</v>
       </c>
       <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -2421,10 +2628,13 @@
         <v>148</v>
       </c>
       <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -2436,10 +2646,13 @@
         <v>149</v>
       </c>
       <c r="D71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -2451,10 +2664,13 @@
         <v>150</v>
       </c>
       <c r="D72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -2466,10 +2682,13 @@
         <v>151</v>
       </c>
       <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -2481,10 +2700,13 @@
         <v>152</v>
       </c>
       <c r="D74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2496,10 +2718,13 @@
         <v>153</v>
       </c>
       <c r="D75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2511,7 +2736,10 @@
         <v>154</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>